<commit_message>
Updated get balance button
</commit_message>
<xml_diff>
--- a/saldo.xlsx
+++ b/saldo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>nome moeda</t>
   </si>
@@ -25,13 +25,34 @@
     <t>GAL</t>
   </si>
   <si>
-    <t>asdasjd</t>
+    <t>SHIB</t>
+  </si>
+  <si>
+    <t>FIRO</t>
+  </si>
+  <si>
+    <t>SOL</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>ADA</t>
+  </si>
+  <si>
+    <t>XRP</t>
+  </si>
+  <si>
+    <t>USDT</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>BTC</t>
   </si>
   <si>
     <t>2.57941800</t>
-  </si>
-  <si>
-    <t>asdjasd</t>
   </si>
 </sst>
 </file>
@@ -389,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,7 +432,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -421,8 +442,8 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="C3">
+        <v>1307702.99</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -430,10 +451,87 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
         <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0.08190859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>0.36963</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1.14509252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>33.7662</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>172.790793</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>0.0022175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.00945705</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>6.1E-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>